<commit_message>
new feature: Offline mode
</commit_message>
<xml_diff>
--- a/coordinates.xlsx
+++ b/coordinates.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11835" windowWidth="21600" xWindow="5370" yWindow="2040"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="16440" windowWidth="29040" xWindow="-120" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="ANLIOSTASIO" sheetId="1" state="visible" r:id="rId1"/>
@@ -391,7 +391,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="J3:K13"/>
+      <selection activeCell="H3" sqref="H3:K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -458,6 +458,24 @@
       <c r="A3" t="n">
         <v>1</v>
       </c>
+      <c r="B3" t="n">
+        <v>40</v>
+      </c>
+      <c r="C3" t="n">
+        <v>31</v>
+      </c>
+      <c r="D3" t="n">
+        <v>24.49</v>
+      </c>
+      <c r="E3" t="n">
+        <v>21</v>
+      </c>
+      <c r="F3" t="n">
+        <v>41</v>
+      </c>
+      <c r="G3" t="n">
+        <v>4.34</v>
+      </c>
       <c r="H3" t="inlineStr">
         <is>
           <t>40.52346944</t>
@@ -483,6 +501,24 @@
       <c r="A4" t="n">
         <v>2</v>
       </c>
+      <c r="B4" t="n">
+        <v>40</v>
+      </c>
+      <c r="C4" t="n">
+        <v>31</v>
+      </c>
+      <c r="D4" t="n">
+        <v>24.21</v>
+      </c>
+      <c r="E4" t="n">
+        <v>21</v>
+      </c>
+      <c r="F4" t="n">
+        <v>41</v>
+      </c>
+      <c r="G4" t="n">
+        <v>4.38</v>
+      </c>
       <c r="H4" t="inlineStr">
         <is>
           <t>40.52339167</t>
@@ -508,6 +544,24 @@
       <c r="A5" t="n">
         <v>3</v>
       </c>
+      <c r="B5" t="n">
+        <v>40</v>
+      </c>
+      <c r="C5" t="n">
+        <v>31</v>
+      </c>
+      <c r="D5" t="n">
+        <v>24.19</v>
+      </c>
+      <c r="E5" t="n">
+        <v>21</v>
+      </c>
+      <c r="F5" t="n">
+        <v>41</v>
+      </c>
+      <c r="G5" t="n">
+        <v>4.15</v>
+      </c>
       <c r="H5" t="inlineStr">
         <is>
           <t>40.52338611</t>
@@ -533,6 +587,24 @@
       <c r="A6" t="n">
         <v>4</v>
       </c>
+      <c r="B6" t="n">
+        <v>40</v>
+      </c>
+      <c r="C6" t="n">
+        <v>31</v>
+      </c>
+      <c r="D6" t="n">
+        <v>25.85</v>
+      </c>
+      <c r="E6" t="n">
+        <v>21</v>
+      </c>
+      <c r="F6" t="n">
+        <v>40</v>
+      </c>
+      <c r="G6" t="n">
+        <v>59.87</v>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
           <t>40.52384722</t>
@@ -545,12 +617,12 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>303607.77423981</t>
+          <t>303707.14658056</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>4488194.4349555</t>
+          <t>4488140.5979287</t>
         </is>
       </c>
     </row>
@@ -558,6 +630,24 @@
       <c r="A7" t="n">
         <v>5</v>
       </c>
+      <c r="B7" t="n">
+        <v>40</v>
+      </c>
+      <c r="C7" t="n">
+        <v>31</v>
+      </c>
+      <c r="D7" t="n">
+        <v>25.73</v>
+      </c>
+      <c r="E7" t="n">
+        <v>21</v>
+      </c>
+      <c r="F7" t="n">
+        <v>40</v>
+      </c>
+      <c r="G7" t="n">
+        <v>59.84</v>
+      </c>
       <c r="H7" t="inlineStr">
         <is>
           <t>40.52381389</t>
@@ -570,12 +660,12 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>303606.97129996</t>
+          <t>303607.77423981</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>4488190.7533626</t>
+          <t>4488194.4349555</t>
         </is>
       </c>
     </row>
@@ -583,6 +673,24 @@
       <c r="A8" t="n">
         <v>6</v>
       </c>
+      <c r="B8" t="n">
+        <v>40</v>
+      </c>
+      <c r="C8" t="n">
+        <v>31</v>
+      </c>
+      <c r="D8" t="n">
+        <v>25.72</v>
+      </c>
+      <c r="E8" t="n">
+        <v>21</v>
+      </c>
+      <c r="F8" t="n">
+        <v>40</v>
+      </c>
+      <c r="G8" t="n">
+        <v>59.71</v>
+      </c>
       <c r="H8" t="inlineStr">
         <is>
           <t>40.52381111</t>
@@ -595,12 +703,12 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>303603.90411498</t>
+          <t>303607.77423981</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>4488190.5251506</t>
+          <t>4488194.4349555</t>
         </is>
       </c>
     </row>
@@ -608,6 +716,24 @@
       <c r="A9" t="n">
         <v>7</v>
       </c>
+      <c r="B9" t="n">
+        <v>40</v>
+      </c>
+      <c r="C9" t="n">
+        <v>31</v>
+      </c>
+      <c r="D9" t="n">
+        <v>25.63</v>
+      </c>
+      <c r="E9" t="n">
+        <v>21</v>
+      </c>
+      <c r="F9" t="n">
+        <v>40</v>
+      </c>
+      <c r="G9" t="n">
+        <v>59.71</v>
+      </c>
       <c r="H9" t="inlineStr">
         <is>
           <t>40.52378611</t>
@@ -620,12 +746,12 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>303603.8311608</t>
+          <t>303606.97129996</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>4488187.7497665</t>
+          <t>4488190.7533626</t>
         </is>
       </c>
     </row>
@@ -633,6 +759,24 @@
       <c r="A10" t="n">
         <v>8</v>
       </c>
+      <c r="B10" t="n">
+        <v>40</v>
+      </c>
+      <c r="C10" t="n">
+        <v>31</v>
+      </c>
+      <c r="D10" t="n">
+        <v>25.52</v>
+      </c>
+      <c r="E10" t="n">
+        <v>21</v>
+      </c>
+      <c r="F10" t="n">
+        <v>40</v>
+      </c>
+      <c r="G10" t="n">
+        <v>59.74</v>
+      </c>
       <c r="H10" t="inlineStr">
         <is>
           <t>40.52375556</t>
@@ -645,12 +789,12 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>303604.4476906</t>
+          <t>303606.97129996</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>4488184.3396975</t>
+          <t>4488190.7533626</t>
         </is>
       </c>
     </row>
@@ -658,6 +802,24 @@
       <c r="A11" t="n">
         <v>9</v>
       </c>
+      <c r="B11" t="n">
+        <v>40</v>
+      </c>
+      <c r="C11" t="n">
+        <v>31</v>
+      </c>
+      <c r="D11" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="E11" t="n">
+        <v>21</v>
+      </c>
+      <c r="F11" t="n">
+        <v>40</v>
+      </c>
+      <c r="G11" t="n">
+        <v>59.7</v>
+      </c>
       <c r="H11" t="inlineStr">
         <is>
           <t>40.52375000</t>
@@ -670,12 +832,12 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>303603.49027687</t>
+          <t>303606.97129996</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>4488183.7471923</t>
+          <t>4488190.7533626</t>
         </is>
       </c>
     </row>
@@ -683,6 +845,24 @@
       <c r="A12" t="n">
         <v>10</v>
       </c>
+      <c r="B12" t="n">
+        <v>40</v>
+      </c>
+      <c r="C12" t="n">
+        <v>31</v>
+      </c>
+      <c r="D12" t="n">
+        <v>24.27</v>
+      </c>
+      <c r="E12" t="n">
+        <v>21</v>
+      </c>
+      <c r="F12" t="n">
+        <v>40</v>
+      </c>
+      <c r="G12" t="n">
+        <v>59.45</v>
+      </c>
       <c r="H12" t="inlineStr">
         <is>
           <t>40.52340833</t>
@@ -695,12 +875,12 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>303596.61055826</t>
+          <t>303606.97129996</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>4488145.9712079</t>
+          <t>4488190.7533626</t>
         </is>
       </c>
     </row>
@@ -708,6 +888,24 @@
       <c r="A13" t="n">
         <v>11</v>
       </c>
+      <c r="B13" t="n">
+        <v>40</v>
+      </c>
+      <c r="C13" t="n">
+        <v>31</v>
+      </c>
+      <c r="D13" t="n">
+        <v>24.27</v>
+      </c>
+      <c r="E13" t="n">
+        <v>21</v>
+      </c>
+      <c r="F13" t="n">
+        <v>40</v>
+      </c>
+      <c r="G13" t="n">
+        <v>59.36</v>
+      </c>
       <c r="H13" t="inlineStr">
         <is>
           <t>40.52340833</t>
@@ -720,12 +918,12 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>303594.49266088</t>
+          <t>303603.90411498</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>4488146.0268809</t>
+          <t>4488190.5251506</t>
         </is>
       </c>
     </row>

</xml_diff>